<commit_message>
DB new tables added and corresponding constraints
</commit_message>
<xml_diff>
--- a/Database/yelp-lab1-metadata.xlsx
+++ b/Database/yelp-lab1-metadata.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$F$132</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$F$134</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="128">
   <si>
     <t>Entity</t>
   </si>
@@ -66,7 +66,7 @@
     <t>Customer/Resturant</t>
   </si>
   <si>
-    <t>RESTURANT</t>
+    <t>RESTAURANT</t>
   </si>
   <si>
     <t>INT</t>
@@ -75,7 +75,7 @@
     <t>Autoincremented</t>
   </si>
   <si>
-    <t>Resturant_ID</t>
+    <t>Restaurant_ID</t>
   </si>
   <si>
     <t>Generated during Signup</t>
@@ -156,7 +156,7 @@
     <t>Options</t>
   </si>
   <si>
-    <t>DELIVERY_TYPE_RESTURANT_MAPPINGS</t>
+    <t>DELIVERY_TYPE_RESTAURANT_MAPPINGS</t>
   </si>
   <si>
     <t>Delivery_ID</t>
@@ -216,25 +216,25 @@
     <t>VArchar</t>
   </si>
   <si>
-    <t>ResturantImages</t>
+    <t>RESTAURANT_IMAGES</t>
   </si>
   <si>
     <t>Ask to puneet</t>
   </si>
   <si>
-    <t>ResturantId</t>
-  </si>
-  <si>
-    <t>DishesImages</t>
-  </si>
-  <si>
-    <t>MenuCategoryID</t>
+    <t>FOOD_IMAGES</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Menu_Category_Id</t>
   </si>
   <si>
     <t>From MenuCategory</t>
   </si>
   <si>
-    <t>FoodItemId</t>
+    <t>Food_Item_Id</t>
   </si>
   <si>
     <t>From one of the category</t>
@@ -330,7 +330,7 @@
     <t>Hashtags</t>
   </si>
   <si>
-    <t>REGISTERATION</t>
+    <t>REGISTRATION</t>
   </si>
   <si>
     <t>Event_ID</t>
@@ -406,7 +406,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m-d"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -422,6 +422,7 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <sz val="10.0"/>
       <color theme="1"/>
@@ -433,11 +434,18 @@
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10.0"/>
+      <name val="Sans-serif"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
   </fonts>
   <fills count="5">
     <fill>
@@ -454,14 +462,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF0000"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -471,7 +479,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -483,40 +491,46 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -969,7 +983,7 @@
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1356,188 +1370,188 @@
       <c r="Z17" s="4"/>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="6">
         <v>100.0</v>
       </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="3" t="s">
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-      <c r="W18" s="4"/>
-      <c r="X18" s="4"/>
-      <c r="Y18" s="4"/>
-      <c r="Z18" s="4"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="7"/>
     </row>
     <row r="19">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="5" t="s">
+      <c r="D19" s="9"/>
+      <c r="E19" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="5" t="b">
+      <c r="F19" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="6"/>
-      <c r="S19" s="6"/>
-      <c r="T19" s="6"/>
-      <c r="U19" s="6"/>
-      <c r="V19" s="6"/>
-      <c r="W19" s="6"/>
-      <c r="X19" s="6"/>
-      <c r="Y19" s="6"/>
-      <c r="Z19" s="6"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="9"/>
     </row>
     <row r="20">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="8">
         <v>50.0</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="6"/>
-      <c r="S20" s="6"/>
-      <c r="T20" s="6"/>
-      <c r="U20" s="6"/>
-      <c r="V20" s="6"/>
-      <c r="W20" s="6"/>
-      <c r="X20" s="6"/>
-      <c r="Y20" s="6"/>
-      <c r="Z20" s="6"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
+      <c r="Z20" s="9"/>
     </row>
     <row r="21">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="5" t="s">
+      <c r="D21" s="9"/>
+      <c r="E21" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
-      <c r="S21" s="6"/>
-      <c r="T21" s="6"/>
-      <c r="U21" s="6"/>
-      <c r="V21" s="6"/>
-      <c r="W21" s="6"/>
-      <c r="X21" s="6"/>
-      <c r="Y21" s="6"/>
-      <c r="Z21" s="6"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="9"/>
+      <c r="Z21" s="9"/>
     </row>
     <row r="22">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="8">
         <v>50.0</v>
       </c>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="6"/>
-      <c r="S22" s="6"/>
-      <c r="T22" s="6"/>
-      <c r="U22" s="6"/>
-      <c r="V22" s="6"/>
-      <c r="W22" s="6"/>
-      <c r="X22" s="6"/>
-      <c r="Y22" s="6"/>
-      <c r="Z22" s="6"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="9"/>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="9"/>
+      <c r="Z22" s="9"/>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
@@ -1612,7 +1626,7 @@
       <c r="Z24" s="4"/>
     </row>
     <row r="25">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="10" t="s">
         <v>50</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -1652,7 +1666,7 @@
       <c r="Z25" s="4"/>
     </row>
     <row r="26">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="10" t="s">
         <v>50</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -1688,7 +1702,7 @@
       <c r="Z26" s="4"/>
     </row>
     <row r="27">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="10" t="s">
         <v>50</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -1724,10 +1738,10 @@
       <c r="Z27" s="4"/>
     </row>
     <row r="28">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="11" t="s">
         <v>53</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -1762,7 +1776,7 @@
       <c r="Z28" s="4"/>
     </row>
     <row r="29">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="10" t="s">
         <v>50</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -1798,7 +1812,7 @@
       <c r="Z29" s="4"/>
     </row>
     <row r="30">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="10" t="s">
         <v>50</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -1834,7 +1848,7 @@
       <c r="Z30" s="4"/>
     </row>
     <row r="31">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="10" t="s">
         <v>50</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -1870,43 +1884,43 @@
       <c r="Z31" s="4"/>
     </row>
     <row r="32">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="6">
         <v>100.0</v>
       </c>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
-      <c r="S32" s="4"/>
-      <c r="T32" s="4"/>
-      <c r="U32" s="4"/>
-      <c r="V32" s="4"/>
-      <c r="W32" s="4"/>
-      <c r="X32" s="4"/>
-      <c r="Y32" s="4"/>
-      <c r="Z32" s="4"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="7"/>
+      <c r="T32" s="7"/>
+      <c r="U32" s="7"/>
+      <c r="V32" s="7"/>
+      <c r="W32" s="7"/>
+      <c r="X32" s="7"/>
+      <c r="Y32" s="7"/>
+      <c r="Z32" s="7"/>
     </row>
     <row r="33">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="10" t="s">
         <v>61</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -1944,7 +1958,7 @@
       <c r="Z33" s="4"/>
     </row>
     <row r="34">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="10" t="s">
         <v>61</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -1980,7 +1994,7 @@
       <c r="Z34" s="4"/>
     </row>
     <row r="35">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="10" t="s">
         <v>61</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -2016,10 +2030,10 @@
       <c r="Z35" s="4"/>
     </row>
     <row r="36">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="11" t="s">
         <v>53</v>
       </c>
       <c r="C36" s="3" t="s">
@@ -2054,7 +2068,7 @@
       <c r="Z36" s="4"/>
     </row>
     <row r="37">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="10" t="s">
         <v>61</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -2092,7 +2106,7 @@
       <c r="Z37" s="4"/>
     </row>
     <row r="38">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="10" t="s">
         <v>61</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -2126,7 +2140,7 @@
       <c r="Z38" s="4"/>
     </row>
     <row r="39">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="10" t="s">
         <v>61</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -2162,43 +2176,43 @@
       <c r="Z39" s="4"/>
     </row>
     <row r="40">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="6">
         <v>100.0</v>
       </c>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
-      <c r="N40" s="4"/>
-      <c r="O40" s="4"/>
-      <c r="P40" s="4"/>
-      <c r="Q40" s="4"/>
-      <c r="R40" s="4"/>
-      <c r="S40" s="4"/>
-      <c r="T40" s="4"/>
-      <c r="U40" s="4"/>
-      <c r="V40" s="4"/>
-      <c r="W40" s="4"/>
-      <c r="X40" s="4"/>
-      <c r="Y40" s="4"/>
-      <c r="Z40" s="4"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="7"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="7"/>
+      <c r="S40" s="7"/>
+      <c r="T40" s="7"/>
+      <c r="U40" s="7"/>
+      <c r="V40" s="7"/>
+      <c r="W40" s="7"/>
+      <c r="X40" s="7"/>
+      <c r="Y40" s="7"/>
+      <c r="Z40" s="7"/>
     </row>
     <row r="41">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="11" t="s">
         <v>62</v>
       </c>
       <c r="B41" s="3" t="s">
@@ -2236,7 +2250,7 @@
       <c r="Z41" s="4"/>
     </row>
     <row r="42">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="11" t="s">
         <v>62</v>
       </c>
       <c r="B42" s="3" t="s">
@@ -2272,7 +2286,7 @@
       <c r="Z42" s="4"/>
     </row>
     <row r="43">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="11" t="s">
         <v>62</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -2308,10 +2322,10 @@
       <c r="Z43" s="4"/>
     </row>
     <row r="44">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B44" s="11" t="s">
         <v>53</v>
       </c>
       <c r="C44" s="3" t="s">
@@ -2346,7 +2360,7 @@
       <c r="Z44" s="4"/>
     </row>
     <row r="45">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="11" t="s">
         <v>62</v>
       </c>
       <c r="B45" s="3" t="s">
@@ -2382,7 +2396,7 @@
       <c r="Z45" s="4"/>
     </row>
     <row r="46">
-      <c r="A46" s="8" t="s">
+      <c r="A46" s="11" t="s">
         <v>62</v>
       </c>
       <c r="B46" s="3" t="s">
@@ -2416,7 +2430,7 @@
       <c r="Z46" s="4"/>
     </row>
     <row r="47">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="11" t="s">
         <v>62</v>
       </c>
       <c r="B47" s="3" t="s">
@@ -2454,43 +2468,43 @@
       <c r="Z47" s="4"/>
     </row>
     <row r="48">
-      <c r="A48" s="8" t="s">
+      <c r="A48" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D48" s="6">
         <v>100.0</v>
       </c>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
-      <c r="N48" s="4"/>
-      <c r="O48" s="4"/>
-      <c r="P48" s="4"/>
-      <c r="Q48" s="4"/>
-      <c r="R48" s="4"/>
-      <c r="S48" s="4"/>
-      <c r="T48" s="4"/>
-      <c r="U48" s="4"/>
-      <c r="V48" s="4"/>
-      <c r="W48" s="4"/>
-      <c r="X48" s="4"/>
-      <c r="Y48" s="4"/>
-      <c r="Z48" s="4"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7"/>
+      <c r="K48" s="7"/>
+      <c r="L48" s="7"/>
+      <c r="M48" s="7"/>
+      <c r="N48" s="7"/>
+      <c r="O48" s="7"/>
+      <c r="P48" s="7"/>
+      <c r="Q48" s="7"/>
+      <c r="R48" s="7"/>
+      <c r="S48" s="7"/>
+      <c r="T48" s="7"/>
+      <c r="U48" s="7"/>
+      <c r="V48" s="7"/>
+      <c r="W48" s="7"/>
+      <c r="X48" s="7"/>
+      <c r="Y48" s="7"/>
+      <c r="Z48" s="7"/>
     </row>
     <row r="49">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="11" t="s">
         <v>63</v>
       </c>
       <c r="B49" s="3" t="s">
@@ -2528,7 +2542,7 @@
       <c r="Z49" s="4"/>
     </row>
     <row r="50">
-      <c r="A50" s="8" t="s">
+      <c r="A50" s="11" t="s">
         <v>63</v>
       </c>
       <c r="B50" s="3" t="s">
@@ -2564,7 +2578,7 @@
       <c r="Z50" s="4"/>
     </row>
     <row r="51">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="11" t="s">
         <v>63</v>
       </c>
       <c r="B51" s="3" t="s">
@@ -2600,10 +2614,10 @@
       <c r="Z51" s="4"/>
     </row>
     <row r="52">
-      <c r="A52" s="8" t="s">
+      <c r="A52" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" s="11" t="s">
         <v>53</v>
       </c>
       <c r="C52" s="3" t="s">
@@ -2638,7 +2652,7 @@
       <c r="Z52" s="4"/>
     </row>
     <row r="53">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="11" t="s">
         <v>63</v>
       </c>
       <c r="B53" s="3" t="s">
@@ -2674,7 +2688,7 @@
       <c r="Z53" s="4"/>
     </row>
     <row r="54">
-      <c r="A54" s="8" t="s">
+      <c r="A54" s="11" t="s">
         <v>63</v>
       </c>
       <c r="B54" s="3" t="s">
@@ -2708,7 +2722,7 @@
       <c r="Z54" s="4"/>
     </row>
     <row r="55">
-      <c r="A55" s="8" t="s">
+      <c r="A55" s="11" t="s">
         <v>63</v>
       </c>
       <c r="B55" s="3" t="s">
@@ -2746,43 +2760,43 @@
       <c r="Z55" s="4"/>
     </row>
     <row r="56">
-      <c r="A56" s="8" t="s">
+      <c r="A56" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D56" s="3">
+      <c r="D56" s="6">
         <v>100.0</v>
       </c>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4"/>
-      <c r="G56" s="4"/>
-      <c r="H56" s="4"/>
-      <c r="I56" s="4"/>
-      <c r="J56" s="4"/>
-      <c r="K56" s="4"/>
-      <c r="L56" s="4"/>
-      <c r="M56" s="4"/>
-      <c r="N56" s="4"/>
-      <c r="O56" s="4"/>
-      <c r="P56" s="4"/>
-      <c r="Q56" s="4"/>
-      <c r="R56" s="4"/>
-      <c r="S56" s="4"/>
-      <c r="T56" s="4"/>
-      <c r="U56" s="4"/>
-      <c r="V56" s="4"/>
-      <c r="W56" s="4"/>
-      <c r="X56" s="4"/>
-      <c r="Y56" s="4"/>
-      <c r="Z56" s="4"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
+      <c r="I56" s="7"/>
+      <c r="J56" s="7"/>
+      <c r="K56" s="7"/>
+      <c r="L56" s="7"/>
+      <c r="M56" s="7"/>
+      <c r="N56" s="7"/>
+      <c r="O56" s="7"/>
+      <c r="P56" s="7"/>
+      <c r="Q56" s="7"/>
+      <c r="R56" s="7"/>
+      <c r="S56" s="7"/>
+      <c r="T56" s="7"/>
+      <c r="U56" s="7"/>
+      <c r="V56" s="7"/>
+      <c r="W56" s="7"/>
+      <c r="X56" s="7"/>
+      <c r="Y56" s="7"/>
+      <c r="Z56" s="7"/>
     </row>
     <row r="57">
-      <c r="A57" s="7" t="s">
+      <c r="A57" s="10" t="s">
         <v>64</v>
       </c>
       <c r="B57" s="3" t="s">
@@ -2820,10 +2834,10 @@
       <c r="Z57" s="4"/>
     </row>
     <row r="58">
-      <c r="A58" s="7" t="s">
+      <c r="A58" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C58" s="3" t="s">
@@ -2856,7 +2870,7 @@
       <c r="Z58" s="4"/>
     </row>
     <row r="59">
-      <c r="A59" s="7" t="s">
+      <c r="A59" s="10" t="s">
         <v>64</v>
       </c>
       <c r="B59" s="3" t="s">
@@ -2892,10 +2906,10 @@
       <c r="Z59" s="4"/>
     </row>
     <row r="60">
-      <c r="A60" s="7" t="s">
+      <c r="A60" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B60" s="8" t="s">
+      <c r="B60" s="11" t="s">
         <v>53</v>
       </c>
       <c r="C60" s="3" t="s">
@@ -2930,7 +2944,7 @@
       <c r="Z60" s="4"/>
     </row>
     <row r="61">
-      <c r="A61" s="7" t="s">
+      <c r="A61" s="10" t="s">
         <v>64</v>
       </c>
       <c r="B61" s="3" t="s">
@@ -2966,7 +2980,7 @@
       <c r="Z61" s="4"/>
     </row>
     <row r="62">
-      <c r="A62" s="7" t="s">
+      <c r="A62" s="10" t="s">
         <v>64</v>
       </c>
       <c r="B62" s="3" t="s">
@@ -3000,7 +3014,7 @@
       <c r="Z62" s="4"/>
     </row>
     <row r="63">
-      <c r="A63" s="7" t="s">
+      <c r="A63" s="10" t="s">
         <v>64</v>
       </c>
       <c r="B63" s="3" t="s">
@@ -3038,553 +3052,555 @@
       <c r="Z63" s="4"/>
     </row>
     <row r="64">
-      <c r="A64" s="7" t="s">
+      <c r="A64" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C64" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D64" s="3">
+      <c r="D64" s="6">
         <v>100.0</v>
       </c>
-      <c r="E64" s="4"/>
-      <c r="F64" s="4"/>
-      <c r="G64" s="4"/>
-      <c r="H64" s="4"/>
-      <c r="I64" s="4"/>
-      <c r="J64" s="4"/>
-      <c r="K64" s="4"/>
-      <c r="L64" s="4"/>
-      <c r="M64" s="4"/>
-      <c r="N64" s="4"/>
-      <c r="O64" s="4"/>
-      <c r="P64" s="4"/>
-      <c r="Q64" s="4"/>
-      <c r="R64" s="4"/>
-      <c r="S64" s="4"/>
-      <c r="T64" s="4"/>
-      <c r="U64" s="4"/>
-      <c r="V64" s="4"/>
-      <c r="W64" s="4"/>
-      <c r="X64" s="4"/>
-      <c r="Y64" s="4"/>
-      <c r="Z64" s="4"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
+      <c r="I64" s="7"/>
+      <c r="J64" s="7"/>
+      <c r="K64" s="7"/>
+      <c r="L64" s="7"/>
+      <c r="M64" s="7"/>
+      <c r="N64" s="7"/>
+      <c r="O64" s="7"/>
+      <c r="P64" s="7"/>
+      <c r="Q64" s="7"/>
+      <c r="R64" s="7"/>
+      <c r="S64" s="7"/>
+      <c r="T64" s="7"/>
+      <c r="U64" s="7"/>
+      <c r="V64" s="7"/>
+      <c r="W64" s="7"/>
+      <c r="X64" s="7"/>
+      <c r="Y64" s="7"/>
+      <c r="Z64" s="7"/>
     </row>
     <row r="65">
-      <c r="A65" s="9" t="s">
+      <c r="A65" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C65" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5" t="s">
+      <c r="D65" s="8"/>
+      <c r="E65" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F65" s="6"/>
-      <c r="G65" s="6"/>
-      <c r="H65" s="6"/>
-      <c r="I65" s="6"/>
-      <c r="J65" s="6"/>
-      <c r="K65" s="6"/>
-      <c r="L65" s="6"/>
-      <c r="M65" s="6"/>
-      <c r="N65" s="6"/>
-      <c r="O65" s="6"/>
-      <c r="P65" s="6"/>
-      <c r="Q65" s="6"/>
-      <c r="R65" s="6"/>
-      <c r="S65" s="6"/>
-      <c r="T65" s="6"/>
-      <c r="U65" s="6"/>
-      <c r="V65" s="6"/>
-      <c r="W65" s="6"/>
-      <c r="X65" s="6"/>
-      <c r="Y65" s="6"/>
-      <c r="Z65" s="6"/>
+      <c r="F65" s="9"/>
+      <c r="G65" s="9"/>
+      <c r="H65" s="9"/>
+      <c r="I65" s="9"/>
+      <c r="J65" s="9"/>
+      <c r="K65" s="9"/>
+      <c r="L65" s="9"/>
+      <c r="M65" s="9"/>
+      <c r="N65" s="9"/>
+      <c r="O65" s="9"/>
+      <c r="P65" s="9"/>
+      <c r="Q65" s="9"/>
+      <c r="R65" s="9"/>
+      <c r="S65" s="9"/>
+      <c r="T65" s="9"/>
+      <c r="U65" s="9"/>
+      <c r="V65" s="9"/>
+      <c r="W65" s="9"/>
+      <c r="X65" s="9"/>
+      <c r="Y65" s="9"/>
+      <c r="Z65" s="9"/>
     </row>
     <row r="66">
-      <c r="A66" s="9" t="s">
+      <c r="A66" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C66" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D66" s="5">
+      <c r="D66" s="8">
         <v>50.0</v>
       </c>
-      <c r="E66" s="5"/>
-      <c r="F66" s="6"/>
-      <c r="G66" s="6"/>
-      <c r="H66" s="6"/>
-      <c r="I66" s="6"/>
-      <c r="J66" s="6"/>
-      <c r="K66" s="6"/>
-      <c r="L66" s="6"/>
-      <c r="M66" s="6"/>
-      <c r="N66" s="6"/>
-      <c r="O66" s="6"/>
-      <c r="P66" s="6"/>
-      <c r="Q66" s="6"/>
-      <c r="R66" s="6"/>
-      <c r="S66" s="6"/>
-      <c r="T66" s="6"/>
-      <c r="U66" s="6"/>
-      <c r="V66" s="6"/>
-      <c r="W66" s="6"/>
-      <c r="X66" s="6"/>
-      <c r="Y66" s="6"/>
-      <c r="Z66" s="6"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="9"/>
+      <c r="H66" s="9"/>
+      <c r="I66" s="9"/>
+      <c r="J66" s="9"/>
+      <c r="K66" s="9"/>
+      <c r="L66" s="9"/>
+      <c r="M66" s="9"/>
+      <c r="N66" s="9"/>
+      <c r="O66" s="9"/>
+      <c r="P66" s="9"/>
+      <c r="Q66" s="9"/>
+      <c r="R66" s="9"/>
+      <c r="S66" s="9"/>
+      <c r="T66" s="9"/>
+      <c r="U66" s="9"/>
+      <c r="V66" s="9"/>
+      <c r="W66" s="9"/>
+      <c r="X66" s="9"/>
+      <c r="Y66" s="9"/>
+      <c r="Z66" s="9"/>
     </row>
     <row r="67">
-      <c r="A67" s="10" t="s">
+      <c r="A67" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B67" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C67" s="10" t="s">
+      <c r="B67" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D67" s="5"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H67" s="15"/>
+      <c r="I67" s="15"/>
+      <c r="J67" s="15"/>
+      <c r="K67" s="15"/>
+      <c r="L67" s="15"/>
+      <c r="M67" s="15"/>
+      <c r="N67" s="15"/>
+      <c r="O67" s="15"/>
+      <c r="P67" s="15"/>
+      <c r="Q67" s="15"/>
+      <c r="R67" s="15"/>
+      <c r="S67" s="15"/>
+      <c r="T67" s="15"/>
+      <c r="U67" s="15"/>
+      <c r="V67" s="15"/>
+      <c r="W67" s="15"/>
+      <c r="X67" s="15"/>
+      <c r="Y67" s="15"/>
+      <c r="Z67" s="15"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C68" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D67" s="10">
+      <c r="D68" s="5">
+        <v>100.0</v>
+      </c>
+      <c r="E68" s="4"/>
+      <c r="F68" s="15"/>
+      <c r="G68" s="15"/>
+      <c r="H68" s="15"/>
+      <c r="I68" s="15"/>
+      <c r="J68" s="15"/>
+      <c r="K68" s="15"/>
+      <c r="L68" s="15"/>
+      <c r="M68" s="15"/>
+      <c r="N68" s="15"/>
+      <c r="O68" s="15"/>
+      <c r="P68" s="15"/>
+      <c r="Q68" s="15"/>
+      <c r="R68" s="15"/>
+      <c r="S68" s="15"/>
+      <c r="T68" s="15"/>
+      <c r="U68" s="15"/>
+      <c r="V68" s="15"/>
+      <c r="W68" s="15"/>
+      <c r="X68" s="15"/>
+      <c r="Y68" s="15"/>
+      <c r="Z68" s="15"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D69" s="15"/>
+      <c r="E69" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F69" s="15"/>
+      <c r="G69" s="15"/>
+      <c r="H69" s="15"/>
+      <c r="I69" s="15"/>
+      <c r="J69" s="15"/>
+      <c r="K69" s="15"/>
+      <c r="L69" s="15"/>
+      <c r="M69" s="15"/>
+      <c r="N69" s="15"/>
+      <c r="O69" s="15"/>
+      <c r="P69" s="15"/>
+      <c r="Q69" s="15"/>
+      <c r="R69" s="15"/>
+      <c r="S69" s="15"/>
+      <c r="T69" s="15"/>
+      <c r="U69" s="15"/>
+      <c r="V69" s="15"/>
+      <c r="W69" s="15"/>
+      <c r="X69" s="15"/>
+      <c r="Y69" s="15"/>
+      <c r="Z69" s="15"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D70" s="5">
         <v>500.0</v>
       </c>
-      <c r="E67" s="11"/>
-      <c r="F67" s="11"/>
-      <c r="G67" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H67" s="11"/>
-      <c r="I67" s="11"/>
-      <c r="J67" s="11"/>
-      <c r="K67" s="11"/>
-      <c r="L67" s="11"/>
-      <c r="M67" s="11"/>
-      <c r="N67" s="11"/>
-      <c r="O67" s="11"/>
-      <c r="P67" s="11"/>
-      <c r="Q67" s="11"/>
-      <c r="R67" s="11"/>
-      <c r="S67" s="11"/>
-      <c r="T67" s="11"/>
-      <c r="U67" s="11"/>
-      <c r="V67" s="11"/>
-      <c r="W67" s="11"/>
-      <c r="X67" s="11"/>
-      <c r="Y67" s="11"/>
-      <c r="Z67" s="11"/>
-    </row>
-    <row r="68">
-      <c r="A68" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B68" s="10" t="s">
+      <c r="E70" s="15"/>
+      <c r="F70" s="15"/>
+      <c r="G70" s="15"/>
+      <c r="H70" s="15"/>
+      <c r="I70" s="15"/>
+      <c r="J70" s="15"/>
+      <c r="K70" s="15"/>
+      <c r="L70" s="15"/>
+      <c r="M70" s="15"/>
+      <c r="N70" s="15"/>
+      <c r="O70" s="15"/>
+      <c r="P70" s="15"/>
+      <c r="Q70" s="15"/>
+      <c r="R70" s="15"/>
+      <c r="S70" s="15"/>
+      <c r="T70" s="15"/>
+      <c r="U70" s="15"/>
+      <c r="V70" s="15"/>
+      <c r="W70" s="15"/>
+      <c r="X70" s="15"/>
+      <c r="Y70" s="15"/>
+      <c r="Z70" s="15"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C68" s="11"/>
-      <c r="D68" s="11"/>
-      <c r="E68" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F68" s="11"/>
-      <c r="G68" s="11"/>
-      <c r="H68" s="11"/>
-      <c r="I68" s="11"/>
-      <c r="J68" s="11"/>
-      <c r="K68" s="11"/>
-      <c r="L68" s="11"/>
-      <c r="M68" s="11"/>
-      <c r="N68" s="11"/>
-      <c r="O68" s="11"/>
-      <c r="P68" s="11"/>
-      <c r="Q68" s="11"/>
-      <c r="R68" s="11"/>
-      <c r="S68" s="11"/>
-      <c r="T68" s="11"/>
-      <c r="U68" s="11"/>
-      <c r="V68" s="11"/>
-      <c r="W68" s="11"/>
-      <c r="X68" s="11"/>
-      <c r="Y68" s="11"/>
-      <c r="Z68" s="11"/>
-    </row>
-    <row r="69">
-      <c r="A69" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="B69" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C69" s="10" t="s">
+      <c r="B71" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C71" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D69" s="10">
-        <v>500.0</v>
-      </c>
-      <c r="E69" s="11"/>
-      <c r="F69" s="11"/>
-      <c r="G69" s="11"/>
-      <c r="H69" s="11"/>
-      <c r="I69" s="11"/>
-      <c r="J69" s="11"/>
-      <c r="K69" s="11"/>
-      <c r="L69" s="11"/>
-      <c r="M69" s="11"/>
-      <c r="N69" s="11"/>
-      <c r="O69" s="11"/>
-      <c r="P69" s="11"/>
-      <c r="Q69" s="11"/>
-      <c r="R69" s="11"/>
-      <c r="S69" s="11"/>
-      <c r="T69" s="11"/>
-      <c r="U69" s="11"/>
-      <c r="V69" s="11"/>
-      <c r="W69" s="11"/>
-      <c r="X69" s="11"/>
-      <c r="Y69" s="11"/>
-      <c r="Z69" s="11"/>
-    </row>
-    <row r="70">
-      <c r="A70" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="B70" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C70" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D70" s="11"/>
-      <c r="E70" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F70" s="11"/>
-      <c r="G70" s="11"/>
-      <c r="H70" s="11"/>
-      <c r="I70" s="11"/>
-      <c r="J70" s="11"/>
-      <c r="K70" s="11"/>
-      <c r="L70" s="11"/>
-      <c r="M70" s="11"/>
-      <c r="N70" s="11"/>
-      <c r="O70" s="11"/>
-      <c r="P70" s="11"/>
-      <c r="Q70" s="11"/>
-      <c r="R70" s="11"/>
-      <c r="S70" s="11"/>
-      <c r="T70" s="11"/>
-      <c r="U70" s="11"/>
-      <c r="V70" s="11"/>
-      <c r="W70" s="11"/>
-      <c r="X70" s="11"/>
-      <c r="Y70" s="11"/>
-      <c r="Z70" s="11"/>
-    </row>
-    <row r="71">
-      <c r="A71" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="B71" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C71" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D71" s="11"/>
-      <c r="E71" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="F71" s="11"/>
-      <c r="G71" s="11"/>
-      <c r="H71" s="11"/>
-      <c r="I71" s="11"/>
-      <c r="J71" s="11"/>
-      <c r="K71" s="11"/>
-      <c r="L71" s="11"/>
-      <c r="M71" s="11"/>
-      <c r="N71" s="11"/>
-      <c r="O71" s="11"/>
-      <c r="P71" s="11"/>
-      <c r="Q71" s="11"/>
-      <c r="R71" s="11"/>
-      <c r="S71" s="11"/>
-      <c r="T71" s="11"/>
-      <c r="U71" s="11"/>
-      <c r="V71" s="11"/>
-      <c r="W71" s="11"/>
-      <c r="X71" s="11"/>
-      <c r="Y71" s="11"/>
-      <c r="Z71" s="11"/>
+      <c r="D71" s="5">
+        <v>100.0</v>
+      </c>
+      <c r="E71" s="15"/>
+      <c r="F71" s="15"/>
+      <c r="G71" s="15"/>
+      <c r="H71" s="15"/>
+      <c r="I71" s="15"/>
+      <c r="J71" s="15"/>
+      <c r="K71" s="15"/>
+      <c r="L71" s="15"/>
+      <c r="M71" s="15"/>
+      <c r="N71" s="15"/>
+      <c r="O71" s="15"/>
+      <c r="P71" s="15"/>
+      <c r="Q71" s="15"/>
+      <c r="R71" s="15"/>
+      <c r="S71" s="15"/>
+      <c r="T71" s="15"/>
+      <c r="U71" s="15"/>
+      <c r="V71" s="15"/>
+      <c r="W71" s="15"/>
+      <c r="X71" s="15"/>
+      <c r="Y71" s="15"/>
+      <c r="Z71" s="15"/>
     </row>
     <row r="72">
       <c r="A72" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D72" s="6"/>
-      <c r="E72" s="6"/>
-      <c r="F72" s="6"/>
-      <c r="G72" s="6"/>
-      <c r="H72" s="6"/>
-      <c r="I72" s="6"/>
-      <c r="J72" s="6"/>
-      <c r="K72" s="6"/>
-      <c r="L72" s="6"/>
-      <c r="M72" s="6"/>
-      <c r="N72" s="6"/>
-      <c r="O72" s="6"/>
-      <c r="P72" s="6"/>
-      <c r="Q72" s="6"/>
-      <c r="R72" s="6"/>
-      <c r="S72" s="6"/>
-      <c r="T72" s="6"/>
-      <c r="U72" s="6"/>
-      <c r="V72" s="6"/>
-      <c r="W72" s="6"/>
-      <c r="X72" s="6"/>
-      <c r="Y72" s="6"/>
-      <c r="Z72" s="6"/>
+      <c r="D72" s="15"/>
+      <c r="E72" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F72" s="15"/>
+      <c r="G72" s="15"/>
+      <c r="H72" s="15"/>
+      <c r="I72" s="15"/>
+      <c r="J72" s="15"/>
+      <c r="K72" s="15"/>
+      <c r="L72" s="15"/>
+      <c r="M72" s="15"/>
+      <c r="N72" s="15"/>
+      <c r="O72" s="15"/>
+      <c r="P72" s="15"/>
+      <c r="Q72" s="15"/>
+      <c r="R72" s="15"/>
+      <c r="S72" s="15"/>
+      <c r="T72" s="15"/>
+      <c r="U72" s="15"/>
+      <c r="V72" s="15"/>
+      <c r="W72" s="15"/>
+      <c r="X72" s="15"/>
+      <c r="Y72" s="15"/>
+      <c r="Z72" s="15"/>
     </row>
     <row r="73">
       <c r="A73" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D73" s="15"/>
+      <c r="E73" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F73" s="15"/>
+      <c r="G73" s="15"/>
+      <c r="H73" s="15"/>
+      <c r="I73" s="15"/>
+      <c r="J73" s="15"/>
+      <c r="K73" s="15"/>
+      <c r="L73" s="15"/>
+      <c r="M73" s="15"/>
+      <c r="N73" s="15"/>
+      <c r="O73" s="15"/>
+      <c r="P73" s="15"/>
+      <c r="Q73" s="15"/>
+      <c r="R73" s="15"/>
+      <c r="S73" s="15"/>
+      <c r="T73" s="15"/>
+      <c r="U73" s="15"/>
+      <c r="V73" s="15"/>
+      <c r="W73" s="15"/>
+      <c r="X73" s="15"/>
+      <c r="Y73" s="15"/>
+      <c r="Z73" s="15"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B74" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="9"/>
+      <c r="G74" s="9"/>
+      <c r="H74" s="9"/>
+      <c r="I74" s="9"/>
+      <c r="J74" s="9"/>
+      <c r="K74" s="9"/>
+      <c r="L74" s="9"/>
+      <c r="M74" s="9"/>
+      <c r="N74" s="9"/>
+      <c r="O74" s="9"/>
+      <c r="P74" s="9"/>
+      <c r="Q74" s="9"/>
+      <c r="R74" s="9"/>
+      <c r="S74" s="9"/>
+      <c r="T74" s="9"/>
+      <c r="U74" s="9"/>
+      <c r="V74" s="9"/>
+      <c r="W74" s="9"/>
+      <c r="X74" s="9"/>
+      <c r="Y74" s="9"/>
+      <c r="Z74" s="9"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B75" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C73" s="5" t="s">
+      <c r="C75" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D73" s="5">
+      <c r="D75" s="8">
         <v>50.0</v>
       </c>
-      <c r="E73" s="6"/>
-      <c r="F73" s="6"/>
-      <c r="G73" s="6"/>
-      <c r="H73" s="6"/>
-      <c r="I73" s="6"/>
-      <c r="J73" s="6"/>
-      <c r="K73" s="6"/>
-      <c r="L73" s="6"/>
-      <c r="M73" s="6"/>
-      <c r="N73" s="6"/>
-      <c r="O73" s="6"/>
-      <c r="P73" s="6"/>
-      <c r="Q73" s="6"/>
-      <c r="R73" s="6"/>
-      <c r="S73" s="6"/>
-      <c r="T73" s="6"/>
-      <c r="U73" s="6"/>
-      <c r="V73" s="6"/>
-      <c r="W73" s="6"/>
-      <c r="X73" s="6"/>
-      <c r="Y73" s="6"/>
-      <c r="Z73" s="6"/>
-    </row>
-    <row r="74">
-      <c r="A74" s="5" t="s">
+      <c r="E75" s="9"/>
+      <c r="F75" s="9"/>
+      <c r="G75" s="9"/>
+      <c r="H75" s="9"/>
+      <c r="I75" s="9"/>
+      <c r="J75" s="9"/>
+      <c r="K75" s="9"/>
+      <c r="L75" s="9"/>
+      <c r="M75" s="9"/>
+      <c r="N75" s="9"/>
+      <c r="O75" s="9"/>
+      <c r="P75" s="9"/>
+      <c r="Q75" s="9"/>
+      <c r="R75" s="9"/>
+      <c r="S75" s="9"/>
+      <c r="T75" s="9"/>
+      <c r="U75" s="9"/>
+      <c r="V75" s="9"/>
+      <c r="W75" s="9"/>
+      <c r="X75" s="9"/>
+      <c r="Y75" s="9"/>
+      <c r="Z75" s="9"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B76" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C76" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D74" s="6"/>
-      <c r="E74" s="6"/>
-      <c r="F74" s="6"/>
-      <c r="G74" s="6"/>
-      <c r="H74" s="6"/>
-      <c r="I74" s="6"/>
-      <c r="J74" s="6"/>
-      <c r="K74" s="6"/>
-      <c r="L74" s="6"/>
-      <c r="M74" s="6"/>
-      <c r="N74" s="6"/>
-      <c r="O74" s="6"/>
-      <c r="P74" s="6"/>
-      <c r="Q74" s="6"/>
-      <c r="R74" s="6"/>
-      <c r="S74" s="6"/>
-      <c r="T74" s="6"/>
-      <c r="U74" s="6"/>
-      <c r="V74" s="6"/>
-      <c r="W74" s="6"/>
-      <c r="X74" s="6"/>
-      <c r="Y74" s="6"/>
-      <c r="Z74" s="6"/>
-    </row>
-    <row r="75">
-      <c r="A75" s="5" t="s">
+      <c r="D76" s="9"/>
+      <c r="E76" s="9"/>
+      <c r="F76" s="9"/>
+      <c r="G76" s="9"/>
+      <c r="H76" s="9"/>
+      <c r="I76" s="9"/>
+      <c r="J76" s="9"/>
+      <c r="K76" s="9"/>
+      <c r="L76" s="9"/>
+      <c r="M76" s="9"/>
+      <c r="N76" s="9"/>
+      <c r="O76" s="9"/>
+      <c r="P76" s="9"/>
+      <c r="Q76" s="9"/>
+      <c r="R76" s="9"/>
+      <c r="S76" s="9"/>
+      <c r="T76" s="9"/>
+      <c r="U76" s="9"/>
+      <c r="V76" s="9"/>
+      <c r="W76" s="9"/>
+      <c r="X76" s="9"/>
+      <c r="Y76" s="9"/>
+      <c r="Z76" s="9"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B77" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C75" s="5" t="s">
+      <c r="C77" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D75" s="6"/>
-      <c r="E75" s="5" t="s">
+      <c r="D77" s="9"/>
+      <c r="E77" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="F75" s="6"/>
-      <c r="G75" s="6"/>
-      <c r="H75" s="6"/>
-      <c r="I75" s="6"/>
-      <c r="J75" s="6"/>
-      <c r="K75" s="6"/>
-      <c r="L75" s="6"/>
-      <c r="M75" s="6"/>
-      <c r="N75" s="6"/>
-      <c r="O75" s="6"/>
-      <c r="P75" s="6"/>
-      <c r="Q75" s="6"/>
-      <c r="R75" s="6"/>
-      <c r="S75" s="6"/>
-      <c r="T75" s="6"/>
-      <c r="U75" s="6"/>
-      <c r="V75" s="6"/>
-      <c r="W75" s="6"/>
-      <c r="X75" s="6"/>
-      <c r="Y75" s="6"/>
-      <c r="Z75" s="6"/>
-    </row>
-    <row r="76">
-      <c r="A76" s="5" t="s">
+      <c r="F77" s="9"/>
+      <c r="G77" s="9"/>
+      <c r="H77" s="9"/>
+      <c r="I77" s="9"/>
+      <c r="J77" s="9"/>
+      <c r="K77" s="9"/>
+      <c r="L77" s="9"/>
+      <c r="M77" s="9"/>
+      <c r="N77" s="9"/>
+      <c r="O77" s="9"/>
+      <c r="P77" s="9"/>
+      <c r="Q77" s="9"/>
+      <c r="R77" s="9"/>
+      <c r="S77" s="9"/>
+      <c r="T77" s="9"/>
+      <c r="U77" s="9"/>
+      <c r="V77" s="9"/>
+      <c r="W77" s="9"/>
+      <c r="X77" s="9"/>
+      <c r="Y77" s="9"/>
+      <c r="Z77" s="9"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B78" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="C78" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D76" s="5">
+      <c r="D78" s="8">
         <v>50.0</v>
       </c>
-      <c r="E76" s="6"/>
-      <c r="F76" s="6"/>
-      <c r="G76" s="6"/>
-      <c r="H76" s="6"/>
-      <c r="I76" s="6"/>
-      <c r="J76" s="6"/>
-      <c r="K76" s="6"/>
-      <c r="L76" s="6"/>
-      <c r="M76" s="6"/>
-      <c r="N76" s="6"/>
-      <c r="O76" s="6"/>
-      <c r="P76" s="6"/>
-      <c r="Q76" s="6"/>
-      <c r="R76" s="6"/>
-      <c r="S76" s="6"/>
-      <c r="T76" s="6"/>
-      <c r="U76" s="6"/>
-      <c r="V76" s="6"/>
-      <c r="W76" s="6"/>
-      <c r="X76" s="6"/>
-      <c r="Y76" s="6"/>
-      <c r="Z76" s="6"/>
-    </row>
-    <row r="77">
-      <c r="A77" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D77" s="4"/>
-      <c r="E77" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F77" s="4"/>
-      <c r="G77" s="4"/>
-      <c r="H77" s="4"/>
-      <c r="I77" s="4"/>
-      <c r="J77" s="4"/>
-      <c r="K77" s="4"/>
-      <c r="L77" s="4"/>
-      <c r="M77" s="4"/>
-      <c r="N77" s="4"/>
-      <c r="O77" s="4"/>
-      <c r="P77" s="4"/>
-      <c r="Q77" s="4"/>
-      <c r="R77" s="4"/>
-      <c r="S77" s="4"/>
-      <c r="T77" s="4"/>
-      <c r="U77" s="4"/>
-      <c r="V77" s="4"/>
-      <c r="W77" s="4"/>
-      <c r="X77" s="4"/>
-      <c r="Y77" s="4"/>
-      <c r="Z77" s="4"/>
-    </row>
-    <row r="78">
-      <c r="A78" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D78" s="12">
-        <v>43835.0</v>
-      </c>
-      <c r="E78" s="4"/>
-      <c r="F78" s="4"/>
-      <c r="G78" s="4"/>
-      <c r="H78" s="4"/>
-      <c r="I78" s="4"/>
-      <c r="J78" s="4"/>
-      <c r="K78" s="4"/>
-      <c r="L78" s="4"/>
-      <c r="M78" s="4"/>
-      <c r="N78" s="4"/>
-      <c r="O78" s="4"/>
-      <c r="P78" s="4"/>
-      <c r="Q78" s="4"/>
-      <c r="R78" s="4"/>
-      <c r="S78" s="4"/>
-      <c r="T78" s="4"/>
-      <c r="U78" s="4"/>
-      <c r="V78" s="4"/>
-      <c r="W78" s="4"/>
-      <c r="X78" s="4"/>
-      <c r="Y78" s="4"/>
-      <c r="Z78" s="4"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="9"/>
+      <c r="H78" s="9"/>
+      <c r="I78" s="9"/>
+      <c r="J78" s="9"/>
+      <c r="K78" s="9"/>
+      <c r="L78" s="9"/>
+      <c r="M78" s="9"/>
+      <c r="N78" s="9"/>
+      <c r="O78" s="9"/>
+      <c r="P78" s="9"/>
+      <c r="Q78" s="9"/>
+      <c r="R78" s="9"/>
+      <c r="S78" s="9"/>
+      <c r="T78" s="9"/>
+      <c r="U78" s="9"/>
+      <c r="V78" s="9"/>
+      <c r="W78" s="9"/>
+      <c r="X78" s="9"/>
+      <c r="Y78" s="9"/>
+      <c r="Z78" s="9"/>
     </row>
     <row r="79">
       <c r="A79" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>81</v>
+        <v>7</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D79" s="4"/>
-      <c r="E79" s="4"/>
+      <c r="E79" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="F79" s="4"/>
       <c r="G79" s="4"/>
       <c r="H79" s="4"/>
@@ -3612,12 +3628,14 @@
         <v>78</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D80" s="4"/>
+      <c r="D80" s="16">
+        <v>43835.0</v>
+      </c>
       <c r="E80" s="4"/>
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
@@ -3646,10 +3664,10 @@
         <v>78</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>82</v>
+        <v>18</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81" s="4"/>
@@ -3677,21 +3695,17 @@
     </row>
     <row r="82">
       <c r="A82" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>7</v>
+        <v>78</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D82" s="4"/>
-      <c r="E82" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F82" s="3" t="b">
-        <v>1</v>
-      </c>
+      <c r="E82" s="4"/>
+      <c r="F82" s="4"/>
       <c r="G82" s="4"/>
       <c r="H82" s="4"/>
       <c r="I82" s="4"/>
@@ -3715,18 +3729,16 @@
     </row>
     <row r="83">
       <c r="A83" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="D83" s="4"/>
-      <c r="E83" s="3" t="s">
-        <v>84</v>
-      </c>
+      <c r="E83" s="4"/>
       <c r="F83" s="4"/>
       <c r="G83" s="4"/>
       <c r="H83" s="4"/>
@@ -3754,16 +3766,18 @@
         <v>83</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D84" s="4"/>
       <c r="E84" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F84" s="4"/>
+        <v>43</v>
+      </c>
+      <c r="F84" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="G84" s="4"/>
       <c r="H84" s="4"/>
       <c r="I84" s="4"/>
@@ -3790,13 +3804,15 @@
         <v>83</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>82</v>
+        <v>18</v>
       </c>
       <c r="D85" s="4"/>
-      <c r="E85" s="3"/>
+      <c r="E85" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="F85" s="4"/>
       <c r="G85" s="4"/>
       <c r="H85" s="4"/>
@@ -3823,14 +3839,16 @@
       <c r="A86" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B86" s="3" t="s">
-        <v>38</v>
+      <c r="B86" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="D86" s="4"/>
-      <c r="E86" s="3"/>
+      <c r="E86" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="F86" s="4"/>
       <c r="G86" s="4"/>
       <c r="H86" s="4"/>
@@ -3858,15 +3876,13 @@
         <v>83</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D87" s="4"/>
-      <c r="E87" s="3" t="s">
-        <v>87</v>
-      </c>
+      <c r="E87" s="3"/>
       <c r="F87" s="4"/>
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
@@ -3894,15 +3910,13 @@
         <v>83</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="D88" s="4"/>
-      <c r="E88" s="8" t="s">
-        <v>89</v>
-      </c>
+      <c r="E88" s="3"/>
       <c r="F88" s="4"/>
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
@@ -3926,54 +3940,54 @@
       <c r="Z88" s="4"/>
     </row>
     <row r="89">
-      <c r="A89" s="10" t="s">
+      <c r="A89" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B89" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C89" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D89" s="11"/>
-      <c r="E89" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="F89" s="11"/>
-      <c r="G89" s="11"/>
-      <c r="H89" s="11"/>
-      <c r="I89" s="11"/>
-      <c r="J89" s="11"/>
-      <c r="K89" s="11"/>
-      <c r="L89" s="11"/>
-      <c r="M89" s="11"/>
-      <c r="N89" s="11"/>
-      <c r="O89" s="11"/>
-      <c r="P89" s="11"/>
-      <c r="Q89" s="11"/>
-      <c r="R89" s="11"/>
-      <c r="S89" s="11"/>
-      <c r="T89" s="11"/>
-      <c r="U89" s="11"/>
-      <c r="V89" s="11"/>
-      <c r="W89" s="11"/>
-      <c r="X89" s="11"/>
-      <c r="Y89" s="11"/>
-      <c r="Z89" s="11"/>
+      <c r="B89" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D89" s="4"/>
+      <c r="E89" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F89" s="4"/>
+      <c r="G89" s="4"/>
+      <c r="H89" s="4"/>
+      <c r="I89" s="4"/>
+      <c r="J89" s="4"/>
+      <c r="K89" s="4"/>
+      <c r="L89" s="4"/>
+      <c r="M89" s="4"/>
+      <c r="N89" s="4"/>
+      <c r="O89" s="4"/>
+      <c r="P89" s="4"/>
+      <c r="Q89" s="4"/>
+      <c r="R89" s="4"/>
+      <c r="S89" s="4"/>
+      <c r="T89" s="4"/>
+      <c r="U89" s="4"/>
+      <c r="V89" s="4"/>
+      <c r="W89" s="4"/>
+      <c r="X89" s="4"/>
+      <c r="Y89" s="4"/>
+      <c r="Z89" s="4"/>
     </row>
     <row r="90">
       <c r="A90" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>93</v>
+        <v>18</v>
       </c>
       <c r="D90" s="4"/>
-      <c r="E90" s="14" t="s">
-        <v>94</v>
+      <c r="E90" s="11" t="s">
+        <v>89</v>
       </c>
       <c r="F90" s="4"/>
       <c r="G90" s="4"/>
@@ -3998,57 +4012,55 @@
       <c r="Z90" s="4"/>
     </row>
     <row r="91">
-      <c r="A91" s="3" t="s">
+      <c r="A91" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="B91" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D91" s="3">
-        <v>1000.0</v>
-      </c>
-      <c r="E91" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F91" s="4"/>
-      <c r="G91" s="4"/>
-      <c r="H91" s="4"/>
-      <c r="I91" s="4"/>
-      <c r="J91" s="4"/>
-      <c r="K91" s="4"/>
-      <c r="L91" s="4"/>
-      <c r="M91" s="4"/>
-      <c r="N91" s="4"/>
-      <c r="O91" s="4"/>
-      <c r="P91" s="4"/>
-      <c r="Q91" s="4"/>
-      <c r="R91" s="4"/>
-      <c r="S91" s="4"/>
-      <c r="T91" s="4"/>
-      <c r="U91" s="4"/>
-      <c r="V91" s="4"/>
-      <c r="W91" s="4"/>
-      <c r="X91" s="4"/>
-      <c r="Y91" s="4"/>
-      <c r="Z91" s="4"/>
+      <c r="B91" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C91" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D91" s="18"/>
+      <c r="E91" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="F91" s="18"/>
+      <c r="G91" s="18"/>
+      <c r="H91" s="18"/>
+      <c r="I91" s="18"/>
+      <c r="J91" s="18"/>
+      <c r="K91" s="18"/>
+      <c r="L91" s="18"/>
+      <c r="M91" s="18"/>
+      <c r="N91" s="18"/>
+      <c r="O91" s="18"/>
+      <c r="P91" s="18"/>
+      <c r="Q91" s="18"/>
+      <c r="R91" s="18"/>
+      <c r="S91" s="18"/>
+      <c r="T91" s="18"/>
+      <c r="U91" s="18"/>
+      <c r="V91" s="18"/>
+      <c r="W91" s="18"/>
+      <c r="X91" s="18"/>
+      <c r="Y91" s="18"/>
+      <c r="Z91" s="18"/>
     </row>
     <row r="92">
       <c r="A92" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E92" s="3"/>
+        <v>93</v>
+      </c>
+      <c r="D92" s="4"/>
+      <c r="E92" s="20" t="s">
+        <v>94</v>
+      </c>
       <c r="F92" s="4"/>
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
@@ -4072,161 +4084,165 @@
       <c r="Z92" s="4"/>
     </row>
     <row r="93">
-      <c r="A93" s="5" t="s">
+      <c r="A93" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D93" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F93" s="4"/>
+      <c r="G93" s="4"/>
+      <c r="H93" s="4"/>
+      <c r="I93" s="4"/>
+      <c r="J93" s="4"/>
+      <c r="K93" s="4"/>
+      <c r="L93" s="4"/>
+      <c r="M93" s="4"/>
+      <c r="N93" s="4"/>
+      <c r="O93" s="4"/>
+      <c r="P93" s="4"/>
+      <c r="Q93" s="4"/>
+      <c r="R93" s="4"/>
+      <c r="S93" s="4"/>
+      <c r="T93" s="4"/>
+      <c r="U93" s="4"/>
+      <c r="V93" s="4"/>
+      <c r="W93" s="4"/>
+      <c r="X93" s="4"/>
+      <c r="Y93" s="4"/>
+      <c r="Z93" s="4"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E94" s="3"/>
+      <c r="F94" s="4"/>
+      <c r="G94" s="4"/>
+      <c r="H94" s="4"/>
+      <c r="I94" s="4"/>
+      <c r="J94" s="4"/>
+      <c r="K94" s="4"/>
+      <c r="L94" s="4"/>
+      <c r="M94" s="4"/>
+      <c r="N94" s="4"/>
+      <c r="O94" s="4"/>
+      <c r="P94" s="4"/>
+      <c r="Q94" s="4"/>
+      <c r="R94" s="4"/>
+      <c r="S94" s="4"/>
+      <c r="T94" s="4"/>
+      <c r="U94" s="4"/>
+      <c r="V94" s="4"/>
+      <c r="W94" s="4"/>
+      <c r="X94" s="4"/>
+      <c r="Y94" s="4"/>
+      <c r="Z94" s="4"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B93" s="5" t="s">
+      <c r="B95" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C93" s="5" t="s">
+      <c r="C95" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D93" s="6"/>
-      <c r="E93" s="6"/>
-      <c r="F93" s="5" t="s">
+      <c r="D95" s="9"/>
+      <c r="E95" s="9"/>
+      <c r="F95" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="G93" s="6"/>
-      <c r="H93" s="6"/>
-      <c r="I93" s="6"/>
-      <c r="J93" s="6"/>
-      <c r="K93" s="6"/>
-      <c r="L93" s="6"/>
-      <c r="M93" s="6"/>
-      <c r="N93" s="6"/>
-      <c r="O93" s="6"/>
-      <c r="P93" s="6"/>
-      <c r="Q93" s="6"/>
-      <c r="R93" s="6"/>
-      <c r="S93" s="6"/>
-      <c r="T93" s="6"/>
-      <c r="U93" s="6"/>
-      <c r="V93" s="6"/>
-      <c r="W93" s="6"/>
-      <c r="X93" s="6"/>
-      <c r="Y93" s="6"/>
-      <c r="Z93" s="6"/>
-    </row>
-    <row r="94">
-      <c r="A94" s="5" t="s">
+      <c r="G95" s="9"/>
+      <c r="H95" s="9"/>
+      <c r="I95" s="9"/>
+      <c r="J95" s="9"/>
+      <c r="K95" s="9"/>
+      <c r="L95" s="9"/>
+      <c r="M95" s="9"/>
+      <c r="N95" s="9"/>
+      <c r="O95" s="9"/>
+      <c r="P95" s="9"/>
+      <c r="Q95" s="9"/>
+      <c r="R95" s="9"/>
+      <c r="S95" s="9"/>
+      <c r="T95" s="9"/>
+      <c r="U95" s="9"/>
+      <c r="V95" s="9"/>
+      <c r="W95" s="9"/>
+      <c r="X95" s="9"/>
+      <c r="Y95" s="9"/>
+      <c r="Z95" s="9"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B94" s="5" t="s">
+      <c r="B96" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C94" s="5" t="s">
+      <c r="C96" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D94" s="5">
+      <c r="D96" s="8">
         <v>50.0</v>
       </c>
-      <c r="E94" s="6"/>
-      <c r="F94" s="6"/>
-      <c r="G94" s="6"/>
-      <c r="H94" s="6"/>
-      <c r="I94" s="6"/>
-      <c r="J94" s="6"/>
-      <c r="K94" s="6"/>
-      <c r="L94" s="6"/>
-      <c r="M94" s="6"/>
-      <c r="N94" s="6"/>
-      <c r="O94" s="6"/>
-      <c r="P94" s="6"/>
-      <c r="Q94" s="6"/>
-      <c r="R94" s="6"/>
-      <c r="S94" s="6"/>
-      <c r="T94" s="6"/>
-      <c r="U94" s="6"/>
-      <c r="V94" s="6"/>
-      <c r="W94" s="6"/>
-      <c r="X94" s="6"/>
-      <c r="Y94" s="6"/>
-      <c r="Z94" s="6"/>
-    </row>
-    <row r="95">
-      <c r="A95" s="15" t="s">
+      <c r="E96" s="9"/>
+      <c r="F96" s="9"/>
+      <c r="G96" s="9"/>
+      <c r="H96" s="9"/>
+      <c r="I96" s="9"/>
+      <c r="J96" s="9"/>
+      <c r="K96" s="9"/>
+      <c r="L96" s="9"/>
+      <c r="M96" s="9"/>
+      <c r="N96" s="9"/>
+      <c r="O96" s="9"/>
+      <c r="P96" s="9"/>
+      <c r="Q96" s="9"/>
+      <c r="R96" s="9"/>
+      <c r="S96" s="9"/>
+      <c r="T96" s="9"/>
+      <c r="U96" s="9"/>
+      <c r="V96" s="9"/>
+      <c r="W96" s="9"/>
+      <c r="X96" s="9"/>
+      <c r="Y96" s="9"/>
+      <c r="Z96" s="9"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B97" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C95" s="3" t="s">
+      <c r="C97" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D95" s="4"/>
-      <c r="E95" s="3" t="s">
+      <c r="D97" s="4"/>
+      <c r="E97" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F95" s="4"/>
-      <c r="G95" s="4"/>
-      <c r="H95" s="4"/>
-      <c r="I95" s="4"/>
-      <c r="J95" s="4"/>
-      <c r="K95" s="4"/>
-      <c r="L95" s="4"/>
-      <c r="M95" s="4"/>
-      <c r="N95" s="4"/>
-      <c r="O95" s="4"/>
-      <c r="P95" s="4"/>
-      <c r="Q95" s="4"/>
-      <c r="R95" s="4"/>
-      <c r="S95" s="4"/>
-      <c r="T95" s="4"/>
-      <c r="U95" s="4"/>
-      <c r="V95" s="4"/>
-      <c r="W95" s="4"/>
-      <c r="X95" s="4"/>
-      <c r="Y95" s="4"/>
-      <c r="Z95" s="4"/>
-    </row>
-    <row r="96">
-      <c r="A96" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="B96" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C96" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D96" s="4"/>
-      <c r="E96" s="3"/>
-      <c r="F96" s="4"/>
-      <c r="G96" s="4"/>
-      <c r="H96" s="4"/>
-      <c r="I96" s="4"/>
-      <c r="J96" s="4"/>
-      <c r="K96" s="4"/>
-      <c r="L96" s="4"/>
-      <c r="M96" s="4"/>
-      <c r="N96" s="4"/>
-      <c r="O96" s="4"/>
-      <c r="P96" s="4"/>
-      <c r="Q96" s="4"/>
-      <c r="R96" s="4"/>
-      <c r="S96" s="4"/>
-      <c r="T96" s="4"/>
-      <c r="U96" s="4"/>
-      <c r="V96" s="4"/>
-      <c r="W96" s="4"/>
-      <c r="X96" s="4"/>
-      <c r="Y96" s="4"/>
-      <c r="Z96" s="4"/>
-    </row>
-    <row r="97">
-      <c r="A97" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D97" s="3">
-        <v>100.0</v>
-      </c>
-      <c r="E97" s="4"/>
       <c r="F97" s="4"/>
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
@@ -4250,19 +4266,17 @@
       <c r="Z97" s="4"/>
     </row>
     <row r="98">
-      <c r="A98" s="15" t="s">
+      <c r="A98" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B98" s="3" t="s">
-        <v>4</v>
+      <c r="B98" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D98" s="15">
-        <v>100.0</v>
-      </c>
-      <c r="E98" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="D98" s="4"/>
+      <c r="E98" s="3"/>
       <c r="F98" s="4"/>
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
@@ -4286,16 +4300,18 @@
       <c r="Z98" s="4"/>
     </row>
     <row r="99">
-      <c r="A99" s="15" t="s">
+      <c r="A99" s="3" t="s">
         <v>101</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C99" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="D99" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D99" s="3">
+        <v>100.0</v>
+      </c>
       <c r="E99" s="4"/>
       <c r="F99" s="4"/>
       <c r="G99" s="4"/>
@@ -4320,16 +4336,18 @@
       <c r="Z99" s="4"/>
     </row>
     <row r="100">
-      <c r="A100" s="15" t="s">
+      <c r="A100" s="3" t="s">
         <v>101</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C100" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="D100" s="4"/>
+        <v>4</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D100" s="3">
+        <v>100.0</v>
+      </c>
       <c r="E100" s="4"/>
       <c r="F100" s="4"/>
       <c r="G100" s="4"/>
@@ -4354,19 +4372,17 @@
       <c r="Z100" s="4"/>
     </row>
     <row r="101">
-      <c r="A101" s="15" t="s">
+      <c r="A101" s="3" t="s">
         <v>101</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C101" s="15" t="s">
-        <v>18</v>
+        <v>38</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="D101" s="4"/>
-      <c r="E101" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="E101" s="4"/>
       <c r="F101" s="4"/>
       <c r="G101" s="4"/>
       <c r="H101" s="4"/>
@@ -4390,19 +4406,17 @@
       <c r="Z101" s="4"/>
     </row>
     <row r="102">
-      <c r="A102" s="15" t="s">
+      <c r="A102" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B102" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C102" s="15" t="s">
-        <v>18</v>
+      <c r="B102" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="D102" s="4"/>
-      <c r="E102" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="E102" s="4"/>
       <c r="F102" s="4"/>
       <c r="G102" s="4"/>
       <c r="H102" s="4"/>
@@ -4426,19 +4440,19 @@
       <c r="Z102" s="4"/>
     </row>
     <row r="103">
-      <c r="A103" s="15" t="s">
+      <c r="A103" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B103" s="15" t="s">
-        <v>28</v>
+      <c r="B103" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D103" s="15">
-        <v>25.0</v>
-      </c>
-      <c r="E103" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="D103" s="4"/>
+      <c r="E103" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="F103" s="4"/>
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
@@ -4462,17 +4476,19 @@
       <c r="Z103" s="4"/>
     </row>
     <row r="104">
-      <c r="A104" s="15" t="s">
+      <c r="A104" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B104" s="15" t="s">
-        <v>30</v>
+      <c r="B104" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D104" s="4"/>
-      <c r="E104" s="3"/>
+      <c r="E104" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="F104" s="4"/>
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
@@ -4496,17 +4512,17 @@
       <c r="Z104" s="4"/>
     </row>
     <row r="105">
-      <c r="A105" s="15" t="s">
+      <c r="A105" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B105" s="15" t="s">
-        <v>31</v>
+      <c r="B105" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D105" s="15">
-        <v>50.0</v>
+        <v>29</v>
+      </c>
+      <c r="D105" s="3">
+        <v>25.0</v>
       </c>
       <c r="E105" s="4"/>
       <c r="F105" s="4"/>
@@ -4532,19 +4548,17 @@
       <c r="Z105" s="4"/>
     </row>
     <row r="106">
-      <c r="A106" s="15" t="s">
+      <c r="A106" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B106" s="15" t="s">
-        <v>104</v>
+      <c r="B106" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D106" s="15">
-        <v>100.0</v>
-      </c>
-      <c r="E106" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="D106" s="4"/>
+      <c r="E106" s="3"/>
       <c r="F106" s="4"/>
       <c r="G106" s="4"/>
       <c r="H106" s="4"/>
@@ -4568,19 +4582,19 @@
       <c r="Z106" s="4"/>
     </row>
     <row r="107">
-      <c r="A107" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="B107" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="C107" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D107" s="4"/>
-      <c r="E107" s="15" t="s">
-        <v>107</v>
-      </c>
+      <c r="A107" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D107" s="3">
+        <v>50.0</v>
+      </c>
+      <c r="E107" s="4"/>
       <c r="F107" s="4"/>
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
@@ -4604,16 +4618,18 @@
       <c r="Z107" s="4"/>
     </row>
     <row r="108">
-      <c r="A108" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="B108" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="C108" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D108" s="4"/>
+      <c r="A108" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D108" s="3">
+        <v>100.0</v>
+      </c>
       <c r="E108" s="4"/>
       <c r="F108" s="4"/>
       <c r="G108" s="4"/>
@@ -4638,23 +4654,21 @@
       <c r="Z108" s="4"/>
     </row>
     <row r="109">
-      <c r="A109" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="B109" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C109" s="15" t="s">
+      <c r="A109" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C109" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D109" s="4"/>
-      <c r="E109" s="15" t="s">
-        <v>43</v>
+      <c r="E109" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="F109" s="4"/>
-      <c r="G109" s="15" t="s">
-        <v>109</v>
-      </c>
+      <c r="G109" s="4"/>
       <c r="H109" s="4"/>
       <c r="I109" s="4"/>
       <c r="J109" s="4"/>
@@ -4676,19 +4690,17 @@
       <c r="Z109" s="4"/>
     </row>
     <row r="110">
-      <c r="A110" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="B110" s="15" t="s">
+      <c r="A110" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B110" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C110" s="15" t="s">
+      <c r="C110" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D110" s="4"/>
-      <c r="E110" s="15" t="s">
-        <v>21</v>
-      </c>
+      <c r="E110" s="4"/>
       <c r="F110" s="4"/>
       <c r="G110" s="4"/>
       <c r="H110" s="4"/>
@@ -4712,21 +4724,23 @@
       <c r="Z110" s="4"/>
     </row>
     <row r="111">
-      <c r="A111" s="15" t="s">
+      <c r="A111" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B111" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C111" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D111" s="15">
-        <v>50.0</v>
-      </c>
-      <c r="E111" s="4"/>
+      <c r="B111" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D111" s="4"/>
+      <c r="E111" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="F111" s="4"/>
-      <c r="G111" s="4"/>
+      <c r="G111" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="H111" s="4"/>
       <c r="I111" s="4"/>
       <c r="J111" s="4"/>
@@ -4748,19 +4762,19 @@
       <c r="Z111" s="4"/>
     </row>
     <row r="112">
-      <c r="A112" s="15" t="s">
+      <c r="A112" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B112" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="C112" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D112" s="15">
-        <v>50.0</v>
-      </c>
-      <c r="E112" s="4"/>
+      <c r="B112" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D112" s="4"/>
+      <c r="E112" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="F112" s="4"/>
       <c r="G112" s="4"/>
       <c r="H112" s="4"/>
@@ -4784,16 +4798,18 @@
       <c r="Z112" s="4"/>
     </row>
     <row r="113">
-      <c r="A113" s="15" t="s">
+      <c r="A113" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B113" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="C113" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="D113" s="4"/>
+      <c r="B113" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D113" s="3">
+        <v>50.0</v>
+      </c>
       <c r="E113" s="4"/>
       <c r="F113" s="4"/>
       <c r="G113" s="4"/>
@@ -4818,19 +4834,19 @@
       <c r="Z113" s="4"/>
     </row>
     <row r="114">
-      <c r="A114" s="15" t="s">
+      <c r="A114" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B114" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C114" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D114" s="4"/>
-      <c r="E114" s="15" t="s">
-        <v>25</v>
-      </c>
+      <c r="B114" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D114" s="3">
+        <v>50.0</v>
+      </c>
+      <c r="E114" s="4"/>
       <c r="F114" s="4"/>
       <c r="G114" s="4"/>
       <c r="H114" s="4"/>
@@ -4854,19 +4870,17 @@
       <c r="Z114" s="4"/>
     </row>
     <row r="115">
-      <c r="A115" s="15" t="s">
+      <c r="A115" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B115" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C115" s="15" t="s">
-        <v>18</v>
+      <c r="B115" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="D115" s="4"/>
-      <c r="E115" s="15" t="s">
-        <v>27</v>
-      </c>
+      <c r="E115" s="4"/>
       <c r="F115" s="4"/>
       <c r="G115" s="4"/>
       <c r="H115" s="4"/>
@@ -4890,19 +4904,19 @@
       <c r="Z115" s="4"/>
     </row>
     <row r="116">
-      <c r="A116" s="15" t="s">
+      <c r="A116" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B116" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C116" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D116" s="15">
-        <v>25.0</v>
-      </c>
-      <c r="E116" s="4"/>
+      <c r="B116" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D116" s="4"/>
+      <c r="E116" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="F116" s="4"/>
       <c r="G116" s="4"/>
       <c r="H116" s="4"/>
@@ -4926,17 +4940,19 @@
       <c r="Z116" s="4"/>
     </row>
     <row r="117">
-      <c r="A117" s="15" t="s">
+      <c r="A117" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B117" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="C117" s="15" t="s">
+      <c r="B117" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C117" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D117" s="4"/>
-      <c r="E117" s="15"/>
+      <c r="E117" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="F117" s="4"/>
       <c r="G117" s="4"/>
       <c r="H117" s="4"/>
@@ -4960,17 +4976,17 @@
       <c r="Z117" s="4"/>
     </row>
     <row r="118">
-      <c r="A118" s="15" t="s">
+      <c r="A118" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B118" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C118" s="15" t="s">
+      <c r="B118" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C118" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D118" s="15">
-        <v>50.0</v>
+      <c r="D118" s="3">
+        <v>25.0</v>
       </c>
       <c r="E118" s="4"/>
       <c r="F118" s="4"/>
@@ -4996,17 +5012,17 @@
       <c r="Z118" s="4"/>
     </row>
     <row r="119">
-      <c r="A119" s="15" t="s">
+      <c r="A119" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B119" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C119" s="15" t="s">
-        <v>33</v>
+      <c r="B119" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="D119" s="4"/>
-      <c r="E119" s="4"/>
+      <c r="E119" s="3"/>
       <c r="F119" s="4"/>
       <c r="G119" s="4"/>
       <c r="H119" s="4"/>
@@ -5030,19 +5046,19 @@
       <c r="Z119" s="4"/>
     </row>
     <row r="120">
-      <c r="A120" s="15" t="s">
+      <c r="A120" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B120" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C120" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D120" s="4"/>
-      <c r="E120" s="15" t="s">
-        <v>36</v>
-      </c>
+      <c r="B120" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D120" s="3">
+        <v>50.0</v>
+      </c>
+      <c r="E120" s="4"/>
       <c r="F120" s="4"/>
       <c r="G120" s="4"/>
       <c r="H120" s="4"/>
@@ -5066,18 +5082,16 @@
       <c r="Z120" s="4"/>
     </row>
     <row r="121">
-      <c r="A121" s="15" t="s">
+      <c r="A121" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B121" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="C121" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D121" s="15">
-        <v>100.0</v>
-      </c>
+      <c r="B121" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D121" s="4"/>
       <c r="E121" s="4"/>
       <c r="F121" s="4"/>
       <c r="G121" s="4"/>
@@ -5102,101 +5116,101 @@
       <c r="Z121" s="4"/>
     </row>
     <row r="122">
-      <c r="A122" s="16" t="s">
+      <c r="A122" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B122" s="16" t="s">
+      <c r="B122" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D122" s="4"/>
+      <c r="E122" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F122" s="4"/>
+      <c r="G122" s="4"/>
+      <c r="H122" s="4"/>
+      <c r="I122" s="4"/>
+      <c r="J122" s="4"/>
+      <c r="K122" s="4"/>
+      <c r="L122" s="4"/>
+      <c r="M122" s="4"/>
+      <c r="N122" s="4"/>
+      <c r="O122" s="4"/>
+      <c r="P122" s="4"/>
+      <c r="Q122" s="4"/>
+      <c r="R122" s="4"/>
+      <c r="S122" s="4"/>
+      <c r="T122" s="4"/>
+      <c r="U122" s="4"/>
+      <c r="V122" s="4"/>
+      <c r="W122" s="4"/>
+      <c r="X122" s="4"/>
+      <c r="Y122" s="4"/>
+      <c r="Z122" s="4"/>
+    </row>
+    <row r="123">
+      <c r="A123" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D123" s="3">
+        <v>100.0</v>
+      </c>
+      <c r="E123" s="4"/>
+      <c r="F123" s="4"/>
+      <c r="G123" s="4"/>
+      <c r="H123" s="4"/>
+      <c r="I123" s="4"/>
+      <c r="J123" s="4"/>
+      <c r="K123" s="4"/>
+      <c r="L123" s="4"/>
+      <c r="M123" s="4"/>
+      <c r="N123" s="4"/>
+      <c r="O123" s="4"/>
+      <c r="P123" s="4"/>
+      <c r="Q123" s="4"/>
+      <c r="R123" s="4"/>
+      <c r="S123" s="4"/>
+      <c r="T123" s="4"/>
+      <c r="U123" s="4"/>
+      <c r="V123" s="4"/>
+      <c r="W123" s="4"/>
+      <c r="X123" s="4"/>
+      <c r="Y123" s="4"/>
+      <c r="Z123" s="4"/>
+    </row>
+    <row r="124">
+      <c r="A124" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="B124" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="C122" s="16" t="s">
+      <c r="C124" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D122" s="16">
+      <c r="D124" s="17">
         <v>500.0</v>
       </c>
-      <c r="E122" s="16" t="s">
+      <c r="E124" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="F122" s="17"/>
-      <c r="G122" s="16" t="s">
+      <c r="F124" s="18"/>
+      <c r="G124" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="H122" s="17"/>
-      <c r="I122" s="16" t="s">
+      <c r="H124" s="18"/>
+      <c r="I124" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="J122" s="17"/>
-      <c r="K122" s="17"/>
-      <c r="L122" s="17"/>
-      <c r="M122" s="17"/>
-      <c r="N122" s="17"/>
-      <c r="O122" s="17"/>
-      <c r="P122" s="17"/>
-      <c r="Q122" s="17"/>
-      <c r="R122" s="17"/>
-      <c r="S122" s="17"/>
-      <c r="T122" s="17"/>
-      <c r="U122" s="17"/>
-      <c r="V122" s="17"/>
-      <c r="W122" s="17"/>
-      <c r="X122" s="17"/>
-      <c r="Y122" s="17"/>
-      <c r="Z122" s="17"/>
-    </row>
-    <row r="123">
-      <c r="A123" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="B123" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="C123" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D123" s="15">
-        <v>100.0</v>
-      </c>
-      <c r="E123" s="15"/>
-      <c r="F123" s="18"/>
-      <c r="G123" s="15"/>
-      <c r="H123" s="18"/>
-      <c r="I123" s="15"/>
-      <c r="J123" s="18"/>
-      <c r="K123" s="18"/>
-      <c r="L123" s="18"/>
-      <c r="M123" s="18"/>
-      <c r="N123" s="18"/>
-      <c r="O123" s="18"/>
-      <c r="P123" s="18"/>
-      <c r="Q123" s="18"/>
-      <c r="R123" s="18"/>
-      <c r="S123" s="18"/>
-      <c r="T123" s="18"/>
-      <c r="U123" s="18"/>
-      <c r="V123" s="18"/>
-      <c r="W123" s="18"/>
-      <c r="X123" s="18"/>
-      <c r="Y123" s="18"/>
-      <c r="Z123" s="18"/>
-    </row>
-    <row r="124">
-      <c r="A124" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="B124" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="C124" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D124" s="15">
-        <v>100.0</v>
-      </c>
-      <c r="E124" s="15"/>
-      <c r="F124" s="18"/>
-      <c r="G124" s="15"/>
-      <c r="H124" s="18"/>
-      <c r="I124" s="15"/>
       <c r="J124" s="18"/>
       <c r="K124" s="18"/>
       <c r="L124" s="18"/>
@@ -5216,21 +5230,23 @@
       <c r="Z124" s="18"/>
     </row>
     <row r="125">
-      <c r="A125" s="15" t="s">
+      <c r="A125" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B125" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="C125" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="D125" s="4"/>
-      <c r="E125" s="4"/>
+      <c r="B125" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D125" s="3">
+        <v>100.0</v>
+      </c>
+      <c r="E125" s="3"/>
       <c r="F125" s="4"/>
-      <c r="G125" s="4"/>
+      <c r="G125" s="3"/>
       <c r="H125" s="4"/>
-      <c r="I125" s="4"/>
+      <c r="I125" s="3"/>
       <c r="J125" s="4"/>
       <c r="K125" s="4"/>
       <c r="L125" s="4"/>
@@ -5250,23 +5266,23 @@
       <c r="Z125" s="4"/>
     </row>
     <row r="126">
-      <c r="A126" s="15" t="s">
+      <c r="A126" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B126" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="C126" s="15" t="s">
+      <c r="B126" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C126" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D126" s="15">
+      <c r="D126" s="3">
         <v>100.0</v>
       </c>
-      <c r="E126" s="4"/>
+      <c r="E126" s="3"/>
       <c r="F126" s="4"/>
-      <c r="G126" s="4"/>
+      <c r="G126" s="3"/>
       <c r="H126" s="4"/>
-      <c r="I126" s="4"/>
+      <c r="I126" s="3"/>
       <c r="J126" s="4"/>
       <c r="K126" s="4"/>
       <c r="L126" s="4"/>
@@ -5286,18 +5302,16 @@
       <c r="Z126" s="4"/>
     </row>
     <row r="127">
-      <c r="A127" s="15" t="s">
+      <c r="A127" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B127" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C127" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D127" s="15">
-        <v>100.0</v>
-      </c>
+      <c r="B127" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D127" s="4"/>
       <c r="E127" s="4"/>
       <c r="F127" s="4"/>
       <c r="G127" s="4"/>
@@ -5322,199 +5336,271 @@
       <c r="Z127" s="4"/>
     </row>
     <row r="128">
-      <c r="A128" s="16" t="s">
+      <c r="A128" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D128" s="3">
+        <v>100.0</v>
+      </c>
+      <c r="E128" s="4"/>
+      <c r="F128" s="4"/>
+      <c r="G128" s="4"/>
+      <c r="H128" s="4"/>
+      <c r="I128" s="4"/>
+      <c r="J128" s="4"/>
+      <c r="K128" s="4"/>
+      <c r="L128" s="4"/>
+      <c r="M128" s="4"/>
+      <c r="N128" s="4"/>
+      <c r="O128" s="4"/>
+      <c r="P128" s="4"/>
+      <c r="Q128" s="4"/>
+      <c r="R128" s="4"/>
+      <c r="S128" s="4"/>
+      <c r="T128" s="4"/>
+      <c r="U128" s="4"/>
+      <c r="V128" s="4"/>
+      <c r="W128" s="4"/>
+      <c r="X128" s="4"/>
+      <c r="Y128" s="4"/>
+      <c r="Z128" s="4"/>
+    </row>
+    <row r="129">
+      <c r="A129" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D129" s="3">
+        <v>100.0</v>
+      </c>
+      <c r="E129" s="4"/>
+      <c r="F129" s="4"/>
+      <c r="G129" s="4"/>
+      <c r="H129" s="4"/>
+      <c r="I129" s="4"/>
+      <c r="J129" s="4"/>
+      <c r="K129" s="4"/>
+      <c r="L129" s="4"/>
+      <c r="M129" s="4"/>
+      <c r="N129" s="4"/>
+      <c r="O129" s="4"/>
+      <c r="P129" s="4"/>
+      <c r="Q129" s="4"/>
+      <c r="R129" s="4"/>
+      <c r="S129" s="4"/>
+      <c r="T129" s="4"/>
+      <c r="U129" s="4"/>
+      <c r="V129" s="4"/>
+      <c r="W129" s="4"/>
+      <c r="X129" s="4"/>
+      <c r="Y129" s="4"/>
+      <c r="Z129" s="4"/>
+    </row>
+    <row r="130">
+      <c r="A130" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="B128" s="16" t="s">
+      <c r="B130" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="C128" s="16" t="s">
+      <c r="C130" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D128" s="17"/>
-      <c r="E128" s="17"/>
-      <c r="F128" s="17"/>
-      <c r="G128" s="16" t="s">
+      <c r="D130" s="18"/>
+      <c r="E130" s="18"/>
+      <c r="F130" s="18"/>
+      <c r="G130" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="H128" s="17"/>
-      <c r="I128" s="17"/>
-      <c r="J128" s="17"/>
-      <c r="K128" s="17"/>
-      <c r="L128" s="17"/>
-      <c r="M128" s="17"/>
-      <c r="N128" s="17"/>
-      <c r="O128" s="17"/>
-      <c r="P128" s="17"/>
-      <c r="Q128" s="17"/>
-      <c r="R128" s="17"/>
-      <c r="S128" s="17"/>
-      <c r="T128" s="17"/>
-      <c r="U128" s="17"/>
-      <c r="V128" s="17"/>
-      <c r="W128" s="17"/>
-      <c r="X128" s="17"/>
-      <c r="Y128" s="17"/>
-      <c r="Z128" s="17"/>
-    </row>
-    <row r="129">
-      <c r="A129" s="16" t="s">
+      <c r="H130" s="18"/>
+      <c r="I130" s="18"/>
+      <c r="J130" s="18"/>
+      <c r="K130" s="18"/>
+      <c r="L130" s="18"/>
+      <c r="M130" s="18"/>
+      <c r="N130" s="18"/>
+      <c r="O130" s="18"/>
+      <c r="P130" s="18"/>
+      <c r="Q130" s="18"/>
+      <c r="R130" s="18"/>
+      <c r="S130" s="18"/>
+      <c r="T130" s="18"/>
+      <c r="U130" s="18"/>
+      <c r="V130" s="18"/>
+      <c r="W130" s="18"/>
+      <c r="X130" s="18"/>
+      <c r="Y130" s="18"/>
+      <c r="Z130" s="18"/>
+    </row>
+    <row r="131">
+      <c r="A131" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="B129" s="16" t="s">
+      <c r="B131" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="C129" s="16" t="s">
+      <c r="C131" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="D129" s="17"/>
-      <c r="E129" s="17"/>
-      <c r="F129" s="17"/>
-      <c r="G129" s="17"/>
-      <c r="H129" s="17"/>
-      <c r="I129" s="17"/>
-      <c r="J129" s="17"/>
-      <c r="K129" s="17"/>
-      <c r="L129" s="17"/>
-      <c r="M129" s="17"/>
-      <c r="N129" s="17"/>
-      <c r="O129" s="17"/>
-      <c r="P129" s="17"/>
-      <c r="Q129" s="17"/>
-      <c r="R129" s="17"/>
-      <c r="S129" s="17"/>
-      <c r="T129" s="17"/>
-      <c r="U129" s="17"/>
-      <c r="V129" s="17"/>
-      <c r="W129" s="17"/>
-      <c r="X129" s="17"/>
-      <c r="Y129" s="17"/>
-      <c r="Z129" s="17"/>
-    </row>
-    <row r="130">
-      <c r="A130" s="16" t="s">
+      <c r="D131" s="18"/>
+      <c r="E131" s="18"/>
+      <c r="F131" s="18"/>
+      <c r="G131" s="18"/>
+      <c r="H131" s="18"/>
+      <c r="I131" s="18"/>
+      <c r="J131" s="18"/>
+      <c r="K131" s="18"/>
+      <c r="L131" s="18"/>
+      <c r="M131" s="18"/>
+      <c r="N131" s="18"/>
+      <c r="O131" s="18"/>
+      <c r="P131" s="18"/>
+      <c r="Q131" s="18"/>
+      <c r="R131" s="18"/>
+      <c r="S131" s="18"/>
+      <c r="T131" s="18"/>
+      <c r="U131" s="18"/>
+      <c r="V131" s="18"/>
+      <c r="W131" s="18"/>
+      <c r="X131" s="18"/>
+      <c r="Y131" s="18"/>
+      <c r="Z131" s="18"/>
+    </row>
+    <row r="132">
+      <c r="A132" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="B130" s="16" t="s">
+      <c r="B132" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="C130" s="16" t="s">
+      <c r="C132" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D130" s="16">
+      <c r="D132" s="17">
         <v>100.0</v>
       </c>
-      <c r="E130" s="17"/>
-      <c r="F130" s="17"/>
-      <c r="G130" s="17"/>
-      <c r="H130" s="17"/>
-      <c r="I130" s="17"/>
-      <c r="J130" s="17"/>
-      <c r="K130" s="17"/>
-      <c r="L130" s="17"/>
-      <c r="M130" s="17"/>
-      <c r="N130" s="17"/>
-      <c r="O130" s="17"/>
-      <c r="P130" s="17"/>
-      <c r="Q130" s="17"/>
-      <c r="R130" s="17"/>
-      <c r="S130" s="17"/>
-      <c r="T130" s="17"/>
-      <c r="U130" s="17"/>
-      <c r="V130" s="17"/>
-      <c r="W130" s="17"/>
-      <c r="X130" s="17"/>
-      <c r="Y130" s="17"/>
-      <c r="Z130" s="17"/>
-    </row>
-    <row r="131">
-      <c r="A131" s="15" t="s">
+      <c r="E132" s="18"/>
+      <c r="F132" s="18"/>
+      <c r="G132" s="18"/>
+      <c r="H132" s="18"/>
+      <c r="I132" s="18"/>
+      <c r="J132" s="18"/>
+      <c r="K132" s="18"/>
+      <c r="L132" s="18"/>
+      <c r="M132" s="18"/>
+      <c r="N132" s="18"/>
+      <c r="O132" s="18"/>
+      <c r="P132" s="18"/>
+      <c r="Q132" s="18"/>
+      <c r="R132" s="18"/>
+      <c r="S132" s="18"/>
+      <c r="T132" s="18"/>
+      <c r="U132" s="18"/>
+      <c r="V132" s="18"/>
+      <c r="W132" s="18"/>
+      <c r="X132" s="18"/>
+      <c r="Y132" s="18"/>
+      <c r="Z132" s="18"/>
+    </row>
+    <row r="133">
+      <c r="A133" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B131" s="15" t="s">
+      <c r="B133" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C131" s="15" t="s">
+      <c r="C133" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D131" s="4"/>
-      <c r="E131" s="4"/>
-      <c r="F131" s="4"/>
-      <c r="G131" s="4"/>
-      <c r="H131" s="4"/>
-      <c r="I131" s="4"/>
-      <c r="J131" s="4"/>
-      <c r="K131" s="4"/>
-      <c r="L131" s="4"/>
-      <c r="M131" s="4"/>
-      <c r="N131" s="4"/>
-      <c r="O131" s="4"/>
-      <c r="P131" s="4"/>
-      <c r="Q131" s="4"/>
-      <c r="R131" s="4"/>
-      <c r="S131" s="4"/>
-      <c r="T131" s="4"/>
-      <c r="U131" s="4"/>
-      <c r="V131" s="4"/>
-      <c r="W131" s="4"/>
-      <c r="X131" s="4"/>
-      <c r="Y131" s="4"/>
-      <c r="Z131" s="4"/>
-    </row>
-    <row r="132">
-      <c r="A132" s="15" t="s">
+      <c r="D133" s="4"/>
+      <c r="E133" s="4"/>
+      <c r="F133" s="4"/>
+      <c r="G133" s="4"/>
+      <c r="H133" s="4"/>
+      <c r="I133" s="4"/>
+      <c r="J133" s="4"/>
+      <c r="K133" s="4"/>
+      <c r="L133" s="4"/>
+      <c r="M133" s="4"/>
+      <c r="N133" s="4"/>
+      <c r="O133" s="4"/>
+      <c r="P133" s="4"/>
+      <c r="Q133" s="4"/>
+      <c r="R133" s="4"/>
+      <c r="S133" s="4"/>
+      <c r="T133" s="4"/>
+      <c r="U133" s="4"/>
+      <c r="V133" s="4"/>
+      <c r="W133" s="4"/>
+      <c r="X133" s="4"/>
+      <c r="Y133" s="4"/>
+      <c r="Z133" s="4"/>
+    </row>
+    <row r="134">
+      <c r="A134" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B132" s="15" t="s">
+      <c r="B134" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C132" s="15" t="s">
+      <c r="C134" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D132" s="4"/>
-      <c r="E132" s="4"/>
-      <c r="F132" s="4"/>
-      <c r="G132" s="4"/>
-      <c r="H132" s="4"/>
-      <c r="I132" s="4"/>
-      <c r="J132" s="4"/>
-      <c r="K132" s="4"/>
-      <c r="L132" s="4"/>
-      <c r="M132" s="4"/>
-      <c r="N132" s="4"/>
-      <c r="O132" s="4"/>
-      <c r="P132" s="4"/>
-      <c r="Q132" s="4"/>
-      <c r="R132" s="4"/>
-      <c r="S132" s="4"/>
-      <c r="T132" s="4"/>
-      <c r="U132" s="4"/>
-      <c r="V132" s="4"/>
-      <c r="W132" s="4"/>
-      <c r="X132" s="4"/>
-      <c r="Y132" s="4"/>
-      <c r="Z132" s="4"/>
-    </row>
-    <row r="135">
-      <c r="A135" s="6"/>
-      <c r="B135" s="19" t="s">
+      <c r="D134" s="4"/>
+      <c r="E134" s="4"/>
+      <c r="F134" s="4"/>
+      <c r="G134" s="4"/>
+      <c r="H134" s="4"/>
+      <c r="I134" s="4"/>
+      <c r="J134" s="4"/>
+      <c r="K134" s="4"/>
+      <c r="L134" s="4"/>
+      <c r="M134" s="4"/>
+      <c r="N134" s="4"/>
+      <c r="O134" s="4"/>
+      <c r="P134" s="4"/>
+      <c r="Q134" s="4"/>
+      <c r="R134" s="4"/>
+      <c r="S134" s="4"/>
+      <c r="T134" s="4"/>
+      <c r="U134" s="4"/>
+      <c r="V134" s="4"/>
+      <c r="W134" s="4"/>
+      <c r="X134" s="4"/>
+      <c r="Y134" s="4"/>
+      <c r="Z134" s="4"/>
+    </row>
+    <row r="137">
+      <c r="A137" s="9"/>
+      <c r="B137" s="21" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="136">
-      <c r="A136" s="4"/>
-      <c r="B136" s="19" t="s">
+    <row r="138">
+      <c r="A138" s="4"/>
+      <c r="B138" s="21" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="137">
-      <c r="A137" s="11"/>
-      <c r="B137" s="19" t="s">
+    <row r="139">
+      <c r="A139" s="18"/>
+      <c r="B139" s="21" t="s">
         <v>127</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$F$132"/>
+  <autoFilter ref="$A$1:$F$134"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>